<commit_message>
CI: Sync Excel from SVN to Git
</commit_message>
<xml_diff>
--- a/resource/ExcelTables/Building.xlsx
+++ b/resource/ExcelTables/Building.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SVN\ProjectY\trunk\Tables\datasource\ExcelTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5221AC95-DCC5-449C-92D1-9F94E113BC56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D591A4-6DC9-490B-9ED3-1F1A35913351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35570" yWindow="2360" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-29250" yWindow="2440" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="建筑" sheetId="1" r:id="rId1"/>
@@ -97,7 +97,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>30000,30001</t>
+    <t>地表层;地板层</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -453,7 +453,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.25" defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>